<commit_message>
fixed and optimized the confidence algorithms, also check that previous fixes actually worked; adding a simulator for the parameters of the confidence algorithm...
</commit_message>
<xml_diff>
--- a/DataModel/Calleebree - Quality Formula - Simulation.xlsx
+++ b/DataModel/Calleebree - Quality Formula - Simulation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yann\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TechProjects\sql\calleebree-git\DataModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6B59D6B-8630-4AC2-989B-4DE4B4CE4661}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BDC3BF9-4FC7-4D5B-9313-AF2FD232CFE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10710" yWindow="23100" windowWidth="29010" windowHeight="14520" xr2:uid="{1411CD3C-6E30-4DA4-8CCC-8AF715639E5D}"/>
+    <workbookView xWindow="11340" yWindow="23355" windowWidth="29010" windowHeight="14520" xr2:uid="{1411CD3C-6E30-4DA4-8CCC-8AF715639E5D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -71,7 +71,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -116,7 +116,7 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
@@ -436,7 +436,7 @@
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,7 +498,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="1">
-        <f>ATAN((A8-confidence_mid)/confidence_scale) / PI * 100 + 50</f>
+        <f t="shared" ref="B8:B28" si="0">ATAN((A8-confidence_mid)/confidence_scale) / PI * 100 + 50</f>
         <v>13.785131416218938</v>
       </c>
     </row>
@@ -508,197 +508,197 @@
         <v>20</v>
       </c>
       <c r="B9" s="1">
-        <f>ATAN((A9-confidence_mid)/confidence_scale) / PI * 100 + 50</f>
+        <f t="shared" si="0"/>
         <v>16.372387543895996</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
-        <f t="shared" ref="A10:A28" si="0">A9+10</f>
+        <f t="shared" ref="A10:A28" si="1">A9+10</f>
         <v>30</v>
       </c>
       <c r="B10" s="1">
-        <f>ATAN((A10-confidence_mid)/confidence_scale) / PI * 100 + 50</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="B11" s="1">
-        <f>ATAN((A11-confidence_mid)/confidence_scale) / PI * 100 + 50</f>
+        <f t="shared" si="0"/>
         <v>25.270772792990407</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
       <c r="B12" s="1">
-        <f>ATAN((A12-confidence_mid)/confidence_scale) / PI * 100 + 50</f>
+        <f t="shared" si="0"/>
         <v>33.035878896857241</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
       <c r="B13" s="1">
-        <f>ATAN((A13-confidence_mid)/confidence_scale) / PI * 100 + 50</f>
+        <f t="shared" si="0"/>
         <v>43.820038286915661</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>70</v>
       </c>
       <c r="B14" s="1">
-        <f>ATAN((A14-confidence_mid)/confidence_scale) / PI * 100 + 50</f>
+        <f t="shared" si="0"/>
         <v>56.179961713084339</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>80</v>
       </c>
       <c r="B15" s="1">
-        <f>ATAN((A15-confidence_mid)/confidence_scale) / PI * 100 + 50</f>
+        <f t="shared" si="0"/>
         <v>66.964121103142759</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>90</v>
       </c>
       <c r="B16" s="1">
-        <f>ATAN((A16-confidence_mid)/confidence_scale) / PI * 100 + 50</f>
+        <f t="shared" si="0"/>
         <v>74.729227207009586</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="B17" s="1">
-        <f>ATAN((A17-confidence_mid)/confidence_scale) / PI * 100 + 50</f>
+        <f t="shared" si="0"/>
         <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>110</v>
       </c>
       <c r="B18" s="1">
-        <f>ATAN((A18-confidence_mid)/confidence_scale) / PI * 100 + 50</f>
+        <f t="shared" si="0"/>
         <v>83.627612456104004</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>120</v>
       </c>
       <c r="B19" s="1">
-        <f>ATAN((A19-confidence_mid)/confidence_scale) / PI * 100 + 50</f>
+        <f t="shared" si="0"/>
         <v>86.214868583781055</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>130</v>
       </c>
       <c r="B20" s="1">
-        <f>ATAN((A20-confidence_mid)/confidence_scale) / PI * 100 + 50</f>
+        <f t="shared" si="0"/>
         <v>88.12989280203827</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>140</v>
       </c>
       <c r="B21" s="1">
-        <f>ATAN((A21-confidence_mid)/confidence_scale) / PI * 100 + 50</f>
+        <f t="shared" si="0"/>
         <v>89.594782373069847</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>150</v>
       </c>
       <c r="B22" s="1">
-        <f>ATAN((A22-confidence_mid)/confidence_scale) / PI * 100 + 50</f>
+        <f t="shared" si="0"/>
         <v>90.747044534668504</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>160</v>
       </c>
       <c r="B23" s="1">
-        <f>ATAN((A23-confidence_mid)/confidence_scale) / PI * 100 + 50</f>
+        <f t="shared" si="0"/>
         <v>91.674853072480261</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>170</v>
       </c>
       <c r="B24" s="1">
-        <f>ATAN((A24-confidence_mid)/confidence_scale) / PI * 100 + 50</f>
+        <f t="shared" si="0"/>
         <v>92.43676531066302</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>180</v>
       </c>
       <c r="B25" s="1">
-        <f>ATAN((A25-confidence_mid)/confidence_scale) / PI * 100 + 50</f>
+        <f t="shared" si="0"/>
         <v>93.072943100801936</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>190</v>
       </c>
       <c r="B26" s="1">
-        <f>ATAN((A26-confidence_mid)/confidence_scale) / PI * 100 + 50</f>
+        <f t="shared" si="0"/>
         <v>93.611734398290267</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>200</v>
       </c>
       <c r="B27" s="1">
-        <f>ATAN((A27-confidence_mid)/confidence_scale) / PI * 100 + 50</f>
+        <f t="shared" si="0"/>
         <v>94.073662233697007</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>210</v>
       </c>
       <c r="B28" s="1">
-        <f>ATAN((A28-confidence_mid)/confidence_scale) / PI * 100 + 50</f>
+        <f t="shared" si="0"/>
         <v>94.47392029522473</v>
       </c>
     </row>

</xml_diff>